<commit_message>
Update Excel chart in different languages.xlsx
</commit_message>
<xml_diff>
--- a/Excel chart in different languages.xlsx
+++ b/Excel chart in different languages.xlsx
@@ -9,11 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19155" windowHeight="8820"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19155" windowHeight="8820" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sales,Exp - 2018" sheetId="2" r:id="rId1"/>
-    <sheet name="Tabe and BackEnd" sheetId="1" r:id="rId2"/>
+    <sheet name="Table and BackEnd" sheetId="1" r:id="rId2"/>
     <sheet name="Helper" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
@@ -359,7 +359,7 @@
     <c:title>
       <c:tx>
         <c:strRef>
-          <c:f>'Tabe and BackEnd'!$B$4</c:f>
+          <c:f>'Table and BackEnd'!$B$4</c:f>
           <c:strCache>
             <c:ptCount val="1"/>
             <c:pt idx="0">
@@ -410,7 +410,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Tabe and BackEnd'!$B$6</c:f>
+              <c:f>'Table and BackEnd'!$B$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -491,7 +491,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'Tabe and BackEnd'!$A$7:$A$18</c:f>
+              <c:f>'Table and BackEnd'!$A$7:$A$18</c:f>
               <c:strCache>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
@@ -535,7 +535,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Tabe and BackEnd'!$B$7:$B$18</c:f>
+              <c:f>'Table and BackEnd'!$B$7:$B$18</c:f>
               <c:numCache>
                 <c:formatCode>_("$"* #,##0_);_("$"* \(#,##0\);_("$"* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="12"/>
@@ -584,7 +584,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Tabe and BackEnd'!$C$6</c:f>
+              <c:f>'Table and BackEnd'!$C$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -665,7 +665,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'Tabe and BackEnd'!$A$7:$A$18</c:f>
+              <c:f>'Table and BackEnd'!$A$7:$A$18</c:f>
               <c:strCache>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
@@ -709,7 +709,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Tabe and BackEnd'!$C$7:$C$18</c:f>
+              <c:f>'Table and BackEnd'!$C$7:$C$18</c:f>
               <c:numCache>
                 <c:formatCode>_("$"* #,##0_);_("$"* \(#,##0\);_("$"* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="12"/>
@@ -763,11 +763,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="65"/>
-        <c:axId val="-1692852672"/>
-        <c:axId val="-1692872800"/>
+        <c:axId val="1762534064"/>
+        <c:axId val="1762525904"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1692852672"/>
+        <c:axId val="1762534064"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -810,7 +810,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1692872800"/>
+        <c:crossAx val="1762525904"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -818,7 +818,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1692872800"/>
+        <c:axId val="1762525904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -828,7 +828,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1692852672"/>
+        <c:crossAx val="1762534064"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1540,7 +1540,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main">
   <sheetPr codeName="Chart2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetProtection content="1" objects="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1889,8 +1889,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:RU18"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2296,7 +2296,7 @@
     </row>
     <row r="7" spans="1:489" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="str">
-        <f ca="1">INDIRECT(Lang&amp;ROW())</f>
+        <f t="shared" ref="A7:A18" ca="1" si="0">INDIRECT(Lang&amp;ROW())</f>
         <v>January</v>
       </c>
       <c r="B7" s="3">
@@ -2323,7 +2323,7 @@
     </row>
     <row r="8" spans="1:489" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="str">
-        <f ca="1">INDIRECT(Lang&amp;ROW())</f>
+        <f t="shared" ca="1" si="0"/>
         <v>February</v>
       </c>
       <c r="B8" s="3">
@@ -2348,7 +2348,7 @@
     </row>
     <row r="9" spans="1:489" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="str">
-        <f ca="1">INDIRECT(Lang&amp;ROW())</f>
+        <f t="shared" ca="1" si="0"/>
         <v>March</v>
       </c>
       <c r="B9" s="3">
@@ -2373,7 +2373,7 @@
     </row>
     <row r="10" spans="1:489" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="str">
-        <f ca="1">INDIRECT(Lang&amp;ROW())</f>
+        <f t="shared" ca="1" si="0"/>
         <v>April</v>
       </c>
       <c r="B10" s="3">
@@ -2398,7 +2398,7 @@
     </row>
     <row r="11" spans="1:489" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="str">
-        <f ca="1">INDIRECT(Lang&amp;ROW())</f>
+        <f t="shared" ca="1" si="0"/>
         <v>May</v>
       </c>
       <c r="B11" s="3">
@@ -2423,7 +2423,7 @@
     </row>
     <row r="12" spans="1:489" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="str">
-        <f ca="1">INDIRECT(Lang&amp;ROW())</f>
+        <f t="shared" ca="1" si="0"/>
         <v>June</v>
       </c>
       <c r="B12" s="3">
@@ -2448,7 +2448,7 @@
     </row>
     <row r="13" spans="1:489" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="str">
-        <f ca="1">INDIRECT(Lang&amp;ROW())</f>
+        <f t="shared" ca="1" si="0"/>
         <v>July</v>
       </c>
       <c r="B13" s="3">
@@ -2473,7 +2473,7 @@
     </row>
     <row r="14" spans="1:489" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="str">
-        <f ca="1">INDIRECT(Lang&amp;ROW())</f>
+        <f t="shared" ca="1" si="0"/>
         <v>August</v>
       </c>
       <c r="B14" s="3">
@@ -2498,7 +2498,7 @@
     </row>
     <row r="15" spans="1:489" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="str">
-        <f ca="1">INDIRECT(Lang&amp;ROW())</f>
+        <f t="shared" ca="1" si="0"/>
         <v>September</v>
       </c>
       <c r="B15" s="3">
@@ -2523,7 +2523,7 @@
     </row>
     <row r="16" spans="1:489" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="str">
-        <f ca="1">INDIRECT(Lang&amp;ROW())</f>
+        <f t="shared" ca="1" si="0"/>
         <v>October</v>
       </c>
       <c r="B16" s="3">
@@ -2548,7 +2548,7 @@
     </row>
     <row r="17" spans="1:489" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="str">
-        <f ca="1">INDIRECT(Lang&amp;ROW())</f>
+        <f t="shared" ca="1" si="0"/>
         <v>November</v>
       </c>
       <c r="B17" s="3">
@@ -2573,7 +2573,7 @@
     </row>
     <row r="18" spans="1:489" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="str">
-        <f ca="1">INDIRECT(Lang&amp;ROW())</f>
+        <f t="shared" ca="1" si="0"/>
         <v>December</v>
       </c>
       <c r="B18" s="3">

</xml_diff>